<commit_message>
final code to run
</commit_message>
<xml_diff>
--- a/lottery_results.xlsx
+++ b/lottery_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,11 +471,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11397</t>
+          <t>12024</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>11397</v>
+        <v>12024</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -484,12 +484,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Vacuum Cleaner</t>
+          <t>Futura Pressure Cooker</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/static/prizes/vacuum_cleaner.jpg</t>
+          <t>/static/prizes/futura_pressure_cooker.jpg</t>
         </is>
       </c>
     </row>
@@ -499,25 +499,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>12422</t>
+          <t>17227</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>12422</v>
+        <v>17227</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Birendranagar</t>
+          <t>Lumbini - Bhairahawa</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Samsung Washing Machine</t>
+          <t>Futura Pressure Cooker</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>/static/prizes/samsung_washing_machine.jpg</t>
+          <t>/static/prizes/futura_pressure_cooker.jpg</t>
         </is>
       </c>
     </row>
@@ -527,15 +527,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14194</t>
+          <t>11586</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14194</v>
+        <v>11586</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Gandaki</t>
+          <t>Bagmati</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -555,15 +555,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11635</t>
+          <t>13407</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>11635</v>
+        <v>13407</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Bagmati</t>
+          <t>Dang</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -583,25 +583,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10800</t>
+          <t>14451</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10800</v>
+        <v>14451</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sudurpashim</t>
+          <t>Gandaki</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Futura Pressure Cooker</t>
+          <t>Vacuum Cleaner</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>/static/prizes/futura_pressure_cooker.jpg</t>
+          <t>/static/prizes/vacuum_cleaner.jpg</t>
         </is>
       </c>
     </row>
@@ -611,15 +611,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>18758</t>
+          <t>16472</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18758</v>
+        <v>16472</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Janakpur</t>
+          <t>Gandaki</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -639,23 +639,163 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14264</t>
+          <t>11204</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>14264</v>
+        <v>11204</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>Bagmati</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Vacuum Cleaner</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>/static/prizes/vacuum_cleaner.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10343</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>10343</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mu Ka</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Futura Pressure Cooker</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>/static/prizes/futura_pressure_cooker.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13590</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>13590</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Dang</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Vacuum Cleaner</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>/static/prizes/vacuum_cleaner.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>18428</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>18428</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Janakpur</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Samsung Washing Machine</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>/static/prizes/samsung_washing_machine.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14280</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>14280</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Gandaki</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Futura Pressure Cooker</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>/static/prizes/futura_pressure_cooker.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>17124</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>17124</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bagmati</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Futura Pressure Cooker</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
         <is>
           <t>/static/prizes/futura_pressure_cooker.jpg</t>
         </is>

</xml_diff>